<commit_message>
refactor : Read Input from Excel and write output to excel.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shwet\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shwet\git\Dream11CombinationsFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>WK</t>
   </si>
@@ -103,13 +103,25 @@
   </si>
   <si>
     <t>H Patel</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Sr No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,17 +131,25 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Liberation Sans"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,20 +164,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,221 +481,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
         <v>8.5</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1">
         <v>8.5</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8.5</v>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1">
         <v>8.5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>22</v>
       </c>
-      <c r="D4" s="2">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="2">
+      <c r="C12" s="1">
         <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor : Read Input from Excel and write output to excel. (#3)
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shwet\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shwet\git\Dream11CombinationsFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>WK</t>
   </si>
@@ -103,13 +103,25 @@
   </si>
   <si>
     <t>H Patel</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Sr No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,17 +131,25 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Liberation Sans"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,20 +164,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,221 +481,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
         <v>8.5</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1">
         <v>8.5</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8.5</v>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1">
         <v>8.5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2">
-        <v>9.5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>22</v>
       </c>
-      <c r="D4" s="2">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="2">
+      <c r="C12" s="1">
         <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working commit - Sheet wise output
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shwet\git\Dream11CombinationsFinder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r0s0dgv/WalmartProjects/Dream11CombinationsFinder/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51D2EF5-530C-F246-9C8C-ADE978835187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7065" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
-    <sheet name="DC" sheetId="2" r:id="rId2"/>
+    <sheet name="MI" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">MI!$A$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RR!$A$1:$E$12</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>WK</t>
   </si>
@@ -42,69 +47,15 @@
     <t>J Buttler</t>
   </si>
   <si>
-    <t>S Smith</t>
-  </si>
-  <si>
-    <t>B Strokes</t>
-  </si>
-  <si>
-    <t>J Archer</t>
-  </si>
-  <si>
     <t>S Samson</t>
   </si>
   <si>
-    <t>R Uthapppa</t>
-  </si>
-  <si>
-    <t>R Tewatia</t>
-  </si>
-  <si>
-    <t>J Unadkat</t>
-  </si>
-  <si>
-    <t>D Miller</t>
-  </si>
-  <si>
-    <t>M Lomror</t>
-  </si>
-  <si>
-    <t>S Gopal</t>
-  </si>
-  <si>
-    <t>A Carey</t>
-  </si>
-  <si>
-    <t>S Iyer</t>
-  </si>
-  <si>
-    <t>M Stoinis</t>
-  </si>
-  <si>
-    <t>K Rabada</t>
-  </si>
-  <si>
-    <t>P Saw</t>
-  </si>
-  <si>
-    <t>A Patel</t>
-  </si>
-  <si>
     <t>R Ashwin</t>
   </si>
   <si>
-    <t>S Dhawan</t>
-  </si>
-  <si>
-    <t>A Nortje</t>
-  </si>
-  <si>
     <t>S Hetmyer</t>
   </si>
   <si>
-    <t>H Patel</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -115,13 +66,79 @@
   </si>
   <si>
     <t>Sr No</t>
+  </si>
+  <si>
+    <t>include in DreamTeam ?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>I Kishan</t>
+  </si>
+  <si>
+    <t>Y Chahal</t>
+  </si>
+  <si>
+    <t>T Varma</t>
+  </si>
+  <si>
+    <t>J Bumrah</t>
+  </si>
+  <si>
+    <t>T Mills</t>
+  </si>
+  <si>
+    <t>N Saini</t>
+  </si>
+  <si>
+    <t>K Pollard</t>
+  </si>
+  <si>
+    <t>T boult</t>
+  </si>
+  <si>
+    <t>P Krishna</t>
+  </si>
+  <si>
+    <t>T David</t>
+  </si>
+  <si>
+    <t>D Padikal</t>
+  </si>
+  <si>
+    <t>R Parag</t>
+  </si>
+  <si>
+    <t>A Singh</t>
+  </si>
+  <si>
+    <t>M Ashwin</t>
+  </si>
+  <si>
+    <t>Y Jaiswal</t>
+  </si>
+  <si>
+    <t>B Thampi</t>
+  </si>
+  <si>
+    <t>D Sams</t>
+  </si>
+  <si>
+    <t>Rohit Sharma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +154,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +175,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,10 +190,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -173,8 +203,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -202,7 +237,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -480,29 +515,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -514,13 +557,16 @@
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>9.5</v>
@@ -528,41 +574,50 @@
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
         <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8.5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>8.5</v>
@@ -570,197 +625,241 @@
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
         <v>8.5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>12</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1">
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>9</v>
@@ -768,13 +867,16 @@
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
         <v>8.5</v>
@@ -782,41 +884,50 @@
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
         <v>8.5</v>
@@ -824,22 +935,29 @@
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E12" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code cleanup added .gitignore
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r0s0dgv/WalmartProjects/Dream11CombinationsFinder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51D2EF5-530C-F246-9C8C-ADE978835187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D85B18E-D665-6A48-AB09-7EF2CE512318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RR" sheetId="1" r:id="rId1"/>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -817,7 +817,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -953,7 +953,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>